<commit_message>
Massaging data for the excels and enhancing RunIngest to take multople files and complete the upload
</commit_message>
<xml_diff>
--- a/src/main/resources/questions/Words.xlsx
+++ b/src/main/resources/questions/Words.xlsx
@@ -3169,19 +3169,19 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A974" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F747" activeCellId="0" sqref="F747:F997"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0404858299595"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9028340080972"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9311740890688"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7732793522267"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>